<commit_message>
add tests test_number_of_sites, test_days_count_between_dates
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Day of Month</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Site ID</t>
   </si>
   <si>
@@ -38,12 +35,6 @@
   </si>
   <si>
     <t>Average Time Spent on Site</t>
-  </si>
-  <si>
-    <t>2021-01-01</t>
-  </si>
-  <si>
-    <t>2021-01-02</t>
   </si>
   <si>
     <t>site 1</t>
@@ -425,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,423 +444,372 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
       <c r="G2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
       <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
       <c r="F6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="C7">
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>97</v>
       </c>
       <c r="D8">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="E8">
-        <v>74</v>
+        <v>757</v>
       </c>
       <c r="F8">
-        <v>757</v>
+        <v>81</v>
       </c>
       <c r="G8">
-        <v>81</v>
-      </c>
-      <c r="H8">
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
       </c>
       <c r="D9">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E9">
-        <v>90</v>
+        <v>3075</v>
       </c>
       <c r="F9">
-        <v>3075</v>
+        <v>92</v>
       </c>
       <c r="G9">
-        <v>92</v>
-      </c>
-      <c r="H9">
         <v>3.9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
       </c>
       <c r="D10">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="E10">
+        <v>1222</v>
+      </c>
+      <c r="F10">
         <v>29</v>
       </c>
-      <c r="F10">
-        <v>1222</v>
-      </c>
       <c r="G10">
-        <v>29</v>
-      </c>
-      <c r="H10">
         <v>5.1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="E11">
+        <v>649</v>
+      </c>
+      <c r="F11">
         <v>7</v>
       </c>
-      <c r="F11">
-        <v>649</v>
-      </c>
       <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>159</v>
       </c>
       <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1438</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
         <v>159</v>
       </c>
-      <c r="E12">
+      <c r="D13">
         <v>5</v>
       </c>
-      <c r="F12">
-        <v>1438</v>
-      </c>
-      <c r="G12">
+      <c r="E13">
+        <v>870</v>
+      </c>
+      <c r="F13">
         <v>5</v>
       </c>
-      <c r="H12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
-        <v>159</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>870</v>
-      </c>
       <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
         <v>3.6</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
       </c>
       <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
         <v>4</v>
       </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>11</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>661</v>
       </c>
       <c r="D16">
-        <v>661</v>
+        <v>237</v>
       </c>
       <c r="E16">
-        <v>237</v>
+        <v>9586</v>
       </c>
       <c r="F16">
-        <v>9586</v>
+        <v>248</v>
       </c>
       <c r="G16">
-        <v>248</v>
-      </c>
-      <c r="H16">
         <v>1.3</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>589</v>
       </c>
       <c r="D17">
-        <v>589</v>
+        <v>241</v>
       </c>
       <c r="E17">
-        <v>241</v>
+        <v>10902</v>
       </c>
       <c r="F17">
-        <v>10902</v>
+        <v>255</v>
       </c>
       <c r="G17">
-        <v>255</v>
-      </c>
-      <c r="H17">
         <v>1.7</v>
       </c>
     </row>

</xml_diff>